<commit_message>
fixing errors in data
</commit_message>
<xml_diff>
--- a/data/Covid-19_data.xlsx
+++ b/data/Covid-19_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanjosevidal/Google Drive/Projects/Covid-19/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB733346-C0E6-9E42-968C-2F531968592E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9415E2F-ECAB-C44C-A5F1-3152BB13CFCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{239DC1C1-CD2F-1E41-ACCC-2923A4E1825B}"/>
   </bookViews>
@@ -18,16 +18,16 @@
     <sheet name="Importador" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data_Covid!$A$1:$I$343</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data_Covid!$A$1:$I$476</definedName>
     <definedName name="tabula_Actualizacion_36_COVID_19" localSheetId="0">Data_Covid!$A$191:$H$209</definedName>
     <definedName name="tabula_Actualizacion_37_COVID_19" localSheetId="0">Data_Covid!$A$210:$H$228</definedName>
     <definedName name="tabula_Actualizacion_38_COVID_19" localSheetId="0">Data_Covid!$A$229:$G$247</definedName>
-    <definedName name="tabula_Actualizacion_39_COVID_19" localSheetId="0">Data_Covid!$A$248:$G$266</definedName>
-    <definedName name="tabula_Actualizacion_40_COVID_19" localSheetId="0">Data_Covid!$A$267:$H$285</definedName>
-    <definedName name="tabula_Actualizacion_51_COVID_19" localSheetId="0">Data_Covid!$A$286:$H$305</definedName>
+    <definedName name="tabula_Actualizacion_39_COVID_19" localSheetId="0">Data_Covid!$A$248:$G$248</definedName>
+    <definedName name="tabula_Actualizacion_40_COVID_19" localSheetId="0">Data_Covid!$A$249:$H$266</definedName>
+    <definedName name="tabula_Actualizacion_49_COVID_19" localSheetId="2">Importador!$M$25:$Q$43</definedName>
+    <definedName name="tabula_Actualizacion_51_COVID_19" localSheetId="0">Data_Covid!$A$267:$H$286</definedName>
     <definedName name="tabula_Actualizacion_54_COVID_19" localSheetId="2">Importador!$A$1:$I$21</definedName>
     <definedName name="tabula_Actualizacion_55_COVID_19" localSheetId="2">Importador!$A$25:$G$49</definedName>
-    <definedName name="tabula_Actualizacion_61_COVID_19" localSheetId="2">Importador!$L$23:$R$41</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -101,7 +101,18 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="6" xr16:uid="{71219151-F78B-BF43-B203-0C97CB7948C4}" name="tabula-Actualizacion_51_COVID-191" type="6" refreshedVersion="6" deleted="1" background="1" saveData="1">
+  <connection id="6" xr16:uid="{26ABD4B3-6A20-3648-AE5F-2AD58D291F17}" name="tabula-Actualizacion_49_COVID-19" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/juanjosevidal/Downloads/tabula-Actualizacion_49_COVID-19.csv" decimal="," thousands="." comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="7" xr16:uid="{71219151-F78B-BF43-B203-0C97CB7948C4}" name="tabula-Actualizacion_51_COVID-191" type="6" refreshedVersion="6" deleted="1" background="1" saveData="1">
     <textPr sourceFile="/Users/juanjosevidal/Downloads/tabula-Actualizacion_51_COVID-19.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="7">
         <textField/>
@@ -114,7 +125,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="7" xr16:uid="{D4CDB2D8-FB89-5F46-9B42-A119CD287A81}" name="tabula-Actualizacion_54_COVID-19" type="6" refreshedVersion="6" deleted="1" background="1" saveData="1">
+  <connection id="8" xr16:uid="{D4CDB2D8-FB89-5F46-9B42-A119CD287A81}" name="tabula-Actualizacion_54_COVID-19" type="6" refreshedVersion="6" deleted="1" background="1" saveData="1">
     <textPr sourceFile="/Users/juanjosevidal/Downloads/tabula-Actualizacion_54_COVID-19.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="7">
         <textField/>
@@ -127,23 +138,10 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="8" xr16:uid="{4F988ACB-876B-8B42-8D81-3A573859BE92}" name="tabula-Actualizacion_55_COVID-19" type="6" refreshedVersion="6" deleted="1" background="1" saveData="1">
+  <connection id="9" xr16:uid="{4F988ACB-876B-8B42-8D81-3A573859BE92}" name="tabula-Actualizacion_55_COVID-19" type="6" refreshedVersion="6" deleted="1" background="1" saveData="1">
     <textPr sourceFile="/Users/juanjosevidal/Downloads/tabula-Actualizacion_55_COVID-19.csv" decimal="," thousands="." comma="1">
       <textFields count="8">
         <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="9" xr16:uid="{CC71D802-208A-C043-A00F-FEDF7F8E8655}" name="tabula-Actualizacion_61_COVID-19" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/juanjosevidal/Downloads/tabula-Actualizacion_61_COVID-19.csv" decimal="," thousands="." tab="0" comma="1">
-      <textFields count="7">
         <textField/>
         <textField/>
         <textField/>
@@ -158,7 +156,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="63">
   <si>
     <t>CCAA</t>
   </si>
@@ -337,9 +335,6 @@
     <t>Arag√≥n</t>
   </si>
   <si>
-    <t>Castilla La Mancha</t>
-  </si>
-  <si>
     <t>Castilla y Le√≥n</t>
   </si>
   <si>
@@ -356,7 +351,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -393,6 +388,20 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -487,7 +496,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -518,6 +527,9 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -908,8 +920,8 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>118</xdr:row>
-      <xdr:rowOff>74162</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1159933" cy="0"/>
     <xdr:pic>
@@ -1636,8 +1648,8 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>118</xdr:row>
-      <xdr:rowOff>74162</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1159933" cy="0"/>
     <xdr:pic>
@@ -2481,39 +2493,39 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_51_COVID-19" connectionId="6" xr16:uid="{7C33F37E-B5DB-FC43-B1F3-4C6616C92B19}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_39_COVID-19" connectionId="4" xr16:uid="{8635814F-0D08-FC46-A729-F6EBAF32D7F8}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_40_COVID-19" connectionId="5" xr16:uid="{CC7EF425-5489-914D-8A92-0ACAE9CA3B3B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_51_COVID-19" connectionId="7" xr16:uid="{7C33F37E-B5DB-FC43-B1F3-4C6616C92B19}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_36_COVID-19" connectionId="1" xr16:uid="{903EF60C-4201-D145-9FCB-F17FD78E1C76}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_38_COVID-19" connectionId="3" xr16:uid="{95E03C17-AA2B-FD45-8B76-7C96A74FA4E5}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_37_COVID-19" connectionId="2" xr16:uid="{5CFB9376-3EAD-CA4E-AB81-C1BCF8D4FA26}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_39_COVID-19" connectionId="4" xr16:uid="{8635814F-0D08-FC46-A729-F6EBAF32D7F8}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_40_COVID-19" connectionId="5" xr16:uid="{CC7EF425-5489-914D-8A92-0ACAE9CA3B3B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_36_COVID-19" connectionId="1" xr16:uid="{903EF60C-4201-D145-9FCB-F17FD78E1C76}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_61_COVID-19" connectionId="9" xr16:uid="{5FF6A3BA-506D-DD42-BA20-C4C5829E3E10}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_49_COVID-19" connectionId="6" xr16:uid="{59BF418D-27F8-B240-8C7F-1C3E22902B97}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_54_COVID-19" connectionId="7" xr16:uid="{3CB8AD48-40F5-D349-ACB3-ECA65A993340}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_54_COVID-19" connectionId="8" xr16:uid="{3CB8AD48-40F5-D349-ACB3-ECA65A993340}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_55_COVID-19" connectionId="8" xr16:uid="{02F6A1DC-5207-2947-942B-2AF76DEC0006}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tabula-Actualizacion_55_COVID-19" connectionId="9" xr16:uid="{02F6A1DC-5207-2947-942B-2AF76DEC0006}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2816,8 +2828,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:L495"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A273" zoomScale="108" workbookViewId="0">
+      <selection activeCell="B288" sqref="B288"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2862,7 +2874,7 @@
         <v>56</v>
       </c>
       <c r="L1" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -3311,28 +3323,27 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="18">
         <v>1</v>
       </c>
       <c r="C15" s="3">
         <v>43908</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="19">
         <v>1008</v>
       </c>
-      <c r="E15">
-        <v>11.84</v>
-      </c>
-      <c r="G15" s="9">
-        <v>37</v>
-      </c>
-      <c r="H15" s="9">
-        <v>42</v>
-      </c>
-      <c r="I15" s="13"/>
+      <c r="E15" s="19">
+        <v>12</v>
+      </c>
+      <c r="G15" s="18">
+        <v>25</v>
+      </c>
+      <c r="H15" s="19">
+        <v>23</v>
+      </c>
       <c r="J15" t="str">
         <f>IF(C15&gt;DATE(2020,3,22),"Si","No")</f>
         <v>No</v>
@@ -3769,7 +3780,7 @@
         <v>Si</v>
       </c>
       <c r="K26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L26" t="str">
         <f>IF(C26&gt;DATE(2020,3,15),IF(C26&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -3809,7 +3820,7 @@
         <v>Si</v>
       </c>
       <c r="K27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L27" t="str">
         <f>IF(C27&gt;DATE(2020,3,15),IF(C27&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -4262,28 +4273,27 @@
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="18">
         <v>2</v>
       </c>
       <c r="C41" s="3">
         <v>43908</v>
       </c>
-      <c r="D41" s="9">
+      <c r="D41" s="19">
         <v>281</v>
       </c>
-      <c r="E41">
-        <v>21.22</v>
-      </c>
-      <c r="G41" s="9">
-        <v>54</v>
-      </c>
-      <c r="H41" s="9">
-        <v>29</v>
-      </c>
-      <c r="I41" s="3"/>
+      <c r="E41" s="19">
+        <v>21</v>
+      </c>
+      <c r="G41" s="18">
+        <v>14</v>
+      </c>
+      <c r="H41" s="18">
+        <v>15</v>
+      </c>
       <c r="J41" t="str">
         <f>IF(C41&gt;DATE(2020,3,22),"Si","No")</f>
         <v>No</v>
@@ -4720,7 +4730,7 @@
         <v>Si</v>
       </c>
       <c r="K52" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L52" t="str">
         <f>IF(C52&gt;DATE(2020,3,15),IF(C52&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -4760,7 +4770,7 @@
         <v>Si</v>
       </c>
       <c r="K53" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L53" t="str">
         <f>IF(C53&gt;DATE(2020,3,15),IF(C53&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -5213,28 +5223,27 @@
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
+      <c r="A67" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B67">
+      <c r="B67" s="18">
         <v>3</v>
       </c>
       <c r="C67" s="3">
         <v>43908</v>
       </c>
-      <c r="D67" s="9">
+      <c r="D67" s="19">
         <v>292</v>
       </c>
-      <c r="E67">
+      <c r="E67" s="18">
         <v>28.06</v>
       </c>
-      <c r="G67" s="9">
-        <v>33</v>
-      </c>
-      <c r="H67" s="9">
-        <v>55</v>
-      </c>
-      <c r="I67" s="3"/>
+      <c r="G67" s="18">
+        <v>6</v>
+      </c>
+      <c r="H67" s="18">
+        <v>1</v>
+      </c>
       <c r="J67" t="str">
         <f>IF(C67&gt;DATE(2020,3,22),"Si","No")</f>
         <v>No</v>
@@ -5671,7 +5680,7 @@
         <v>Si</v>
       </c>
       <c r="K78" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L78" t="str">
         <f>IF(C78&gt;DATE(2020,3,15),IF(C78&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -5711,7 +5720,7 @@
         <v>Si</v>
       </c>
       <c r="K79" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L79" t="str">
         <f>IF(C79&gt;DATE(2020,3,15),IF(C79&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -6164,28 +6173,27 @@
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
+      <c r="A93" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B93">
+      <c r="B93" s="18">
         <v>4</v>
       </c>
       <c r="C93" s="3">
         <v>43908</v>
       </c>
-      <c r="D93" s="9">
+      <c r="D93" s="19">
         <v>169</v>
       </c>
-      <c r="E93">
+      <c r="E93" s="18">
         <v>14.18</v>
       </c>
-      <c r="G93" s="9">
-        <v>25</v>
-      </c>
-      <c r="H93" s="9">
-        <v>23</v>
-      </c>
-      <c r="I93" s="3"/>
+      <c r="G93" s="18">
+        <v>7</v>
+      </c>
+      <c r="H93" s="18">
+        <v>2</v>
+      </c>
       <c r="J93" t="str">
         <f>IF(C93&gt;DATE(2020,3,22),"Si","No")</f>
         <v>No</v>
@@ -6622,7 +6630,7 @@
         <v>Si</v>
       </c>
       <c r="K104" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L104" t="str">
         <f>IF(C104&gt;DATE(2020,3,15),IF(C104&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -6662,7 +6670,7 @@
         <v>Si</v>
       </c>
       <c r="K105" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L105" t="str">
         <f>IF(C105&gt;DATE(2020,3,15),IF(C105&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -7115,28 +7123,27 @@
       </c>
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A119" t="s">
+      <c r="A119" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B119">
+      <c r="B119" s="18">
         <v>5</v>
       </c>
       <c r="C119" s="3">
         <v>43908</v>
       </c>
-      <c r="D119" s="9">
+      <c r="D119" s="19">
         <v>220</v>
       </c>
-      <c r="E119">
-        <v>9.84</v>
-      </c>
-      <c r="G119" s="9">
-        <v>14</v>
-      </c>
-      <c r="H119" s="9">
-        <v>15</v>
-      </c>
-      <c r="I119" s="3"/>
+      <c r="E119" s="19">
+        <v>10</v>
+      </c>
+      <c r="G119" s="19">
+        <v>23</v>
+      </c>
+      <c r="H119" s="18">
+        <v>3</v>
+      </c>
       <c r="J119" t="str">
         <f>IF(C119&gt;DATE(2020,3,22),"Si","No")</f>
         <v>No</v>
@@ -7573,7 +7580,7 @@
         <v>Si</v>
       </c>
       <c r="K130" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L130" t="str">
         <f>IF(C130&gt;DATE(2020,3,15),IF(C130&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -7613,7 +7620,7 @@
         <v>Si</v>
       </c>
       <c r="K131" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L131" t="str">
         <f>IF(C131&gt;DATE(2020,3,15),IF(C131&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -8066,28 +8073,27 @@
       </c>
     </row>
     <row r="145" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A145" t="s">
+      <c r="A145" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B145">
+      <c r="B145" s="18">
         <v>6</v>
       </c>
       <c r="C145" s="3">
         <v>43908</v>
       </c>
-      <c r="D145" s="9">
+      <c r="D145" s="19">
         <v>83</v>
       </c>
-      <c r="E145">
-        <v>12.56</v>
-      </c>
-      <c r="G145" s="9">
-        <v>6</v>
-      </c>
-      <c r="H145" s="9">
+      <c r="E145" s="19">
+        <v>13</v>
+      </c>
+      <c r="G145" s="19">
+        <v>4</v>
+      </c>
+      <c r="H145" s="18">
         <v>1</v>
       </c>
-      <c r="I145" s="3"/>
       <c r="J145" t="str">
         <f>IF(C145&gt;DATE(2020,3,22),"Si","No")</f>
         <v>No</v>
@@ -8484,7 +8490,7 @@
         <v>Si</v>
       </c>
       <c r="K155" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L155" t="str">
         <f>IF(C155&gt;DATE(2020,3,15),IF(C155&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -8524,7 +8530,7 @@
         <v>Si</v>
       </c>
       <c r="K156" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L156" t="str">
         <f>IF(C156&gt;DATE(2020,3,15),IF(C156&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -8564,7 +8570,7 @@
         <v>Si</v>
       </c>
       <c r="K157" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L157" t="str">
         <f>IF(C157&gt;DATE(2020,3,15),IF(C157&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -9017,28 +9023,27 @@
       </c>
     </row>
     <row r="171" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A171" t="s">
+      <c r="A171" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B171">
+      <c r="B171" s="18">
         <v>7</v>
       </c>
       <c r="C171" s="3">
         <v>43908</v>
       </c>
-      <c r="D171" s="9">
+      <c r="D171" s="18">
         <v>868</v>
       </c>
-      <c r="E171">
-        <v>35.72</v>
-      </c>
-      <c r="G171" s="9">
-        <v>23</v>
-      </c>
-      <c r="H171" s="9">
-        <v>3</v>
-      </c>
-      <c r="I171" s="3"/>
+      <c r="E171" s="19">
+        <v>36</v>
+      </c>
+      <c r="G171" s="18">
+        <v>54</v>
+      </c>
+      <c r="H171" s="19">
+        <v>29</v>
+      </c>
       <c r="J171" t="str">
         <f>IF(C171&gt;DATE(2020,3,22),"Si","No")</f>
         <v>No</v>
@@ -9435,7 +9440,7 @@
         <v>Si</v>
       </c>
       <c r="K181" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L181" t="str">
         <f>IF(C181&gt;DATE(2020,3,15),IF(C181&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -9475,7 +9480,7 @@
         <v>Si</v>
       </c>
       <c r="K182" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L182" t="str">
         <f>IF(C182&gt;DATE(2020,3,15),IF(C182&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -9515,7 +9520,7 @@
         <v>Si</v>
       </c>
       <c r="K183" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L183" t="str">
         <f>IF(C183&gt;DATE(2020,3,15),IF(C183&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -9968,28 +9973,27 @@
       </c>
     </row>
     <row r="197" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A197" t="s">
+      <c r="A197" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B197">
+      <c r="B197" s="18">
         <v>8</v>
       </c>
       <c r="C197" s="3">
         <v>43908</v>
       </c>
-      <c r="D197" s="9">
+      <c r="D197" s="19">
         <v>801</v>
       </c>
-      <c r="E197">
-        <v>38.76</v>
-      </c>
-      <c r="G197" s="9">
-        <v>7</v>
-      </c>
-      <c r="H197" s="9">
-        <v>2</v>
-      </c>
-      <c r="I197" s="3"/>
+      <c r="E197" s="19">
+        <v>39</v>
+      </c>
+      <c r="G197" s="19">
+        <v>37</v>
+      </c>
+      <c r="H197" s="19">
+        <v>42</v>
+      </c>
       <c r="J197" t="str">
         <f>IF(C197&gt;DATE(2020,3,22),"Si","No")</f>
         <v>No</v>
@@ -10386,7 +10390,7 @@
         <v>Si</v>
       </c>
       <c r="K207" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L207" t="str">
         <f>IF(C207&gt;DATE(2020,3,15),IF(C207&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -10426,7 +10430,7 @@
         <v>Si</v>
       </c>
       <c r="K208" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L208" t="str">
         <f>IF(C208&gt;DATE(2020,3,15),IF(C208&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -10466,7 +10470,7 @@
         <v>Si</v>
       </c>
       <c r="K209" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L209" t="str">
         <f>IF(C209&gt;DATE(2020,3,15),IF(C209&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -10920,28 +10924,27 @@
       </c>
     </row>
     <row r="223" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A223" t="s">
+      <c r="A223" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B223">
+      <c r="B223" s="18">
         <v>9</v>
       </c>
       <c r="C223" s="3">
         <v>43908</v>
       </c>
-      <c r="D223" s="9">
+      <c r="D223" s="19">
         <v>2702</v>
       </c>
-      <c r="E223">
-        <v>34.89</v>
-      </c>
-      <c r="G223" s="9">
-        <v>4</v>
-      </c>
-      <c r="H223" s="9">
-        <v>1</v>
-      </c>
-      <c r="I223" s="3"/>
+      <c r="E223" s="19">
+        <v>35</v>
+      </c>
+      <c r="G223" s="19">
+        <v>33</v>
+      </c>
+      <c r="H223" s="19">
+        <v>55</v>
+      </c>
       <c r="J223" t="str">
         <f>IF(C223&gt;DATE(2020,3,22),"Si","No")</f>
         <v>No</v>
@@ -11338,7 +11341,7 @@
         <v>Si</v>
       </c>
       <c r="K233" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L233" t="str">
         <f>IF(C233&gt;DATE(2020,3,15),IF(C233&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -11378,7 +11381,7 @@
         <v>Si</v>
       </c>
       <c r="K234" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L234" t="str">
         <f>IF(C234&gt;DATE(2020,3,15),IF(C234&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -11418,7 +11421,7 @@
         <v>Si</v>
       </c>
       <c r="K235" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L235" t="str">
         <f>IF(C235&gt;DATE(2020,3,15),IF(C235&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -11871,28 +11874,27 @@
       </c>
     </row>
     <row r="249" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A249" s="1" t="s">
+      <c r="A249" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B249">
+      <c r="B249" s="18">
         <v>10</v>
       </c>
       <c r="C249" s="3">
         <v>43908</v>
       </c>
-      <c r="D249" s="9">
+      <c r="D249" s="19">
         <v>921</v>
       </c>
-      <c r="E249">
-        <v>18.03</v>
-      </c>
-      <c r="G249" s="9">
+      <c r="E249" s="19">
+        <v>18</v>
+      </c>
+      <c r="G249" s="19">
         <v>52</v>
       </c>
-      <c r="H249" s="9">
+      <c r="H249" s="19">
         <v>24</v>
       </c>
-      <c r="I249" s="3"/>
       <c r="J249" t="str">
         <f>IF(C249&gt;DATE(2020,3,22),"Si","No")</f>
         <v>No</v>
@@ -12289,7 +12291,7 @@
         <v>Si</v>
       </c>
       <c r="K259" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L259" t="str">
         <f>IF(C259&gt;DATE(2020,3,15),IF(C259&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -12329,7 +12331,7 @@
         <v>Si</v>
       </c>
       <c r="K260" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L260" t="str">
         <f>IF(C260&gt;DATE(2020,3,15),IF(C260&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -12369,7 +12371,7 @@
         <v>Si</v>
       </c>
       <c r="K261" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L261" t="str">
         <f>IF(C261&gt;DATE(2020,3,15),IF(C261&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -12822,28 +12824,27 @@
       </c>
     </row>
     <row r="275" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A275" t="s">
+      <c r="A275" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B275">
+      <c r="B275" s="18">
         <v>11</v>
       </c>
       <c r="C275" s="3">
         <v>43908</v>
       </c>
-      <c r="D275" s="9">
+      <c r="D275" s="19">
         <v>241</v>
       </c>
-      <c r="E275">
-        <v>22.01</v>
-      </c>
-      <c r="G275" s="9">
+      <c r="E275" s="19">
+        <v>22</v>
+      </c>
+      <c r="G275" s="19">
         <v>3</v>
       </c>
-      <c r="H275" s="9">
+      <c r="H275" s="19">
         <v>8</v>
       </c>
-      <c r="I275" s="3"/>
       <c r="J275" t="str">
         <f>IF(C275&gt;DATE(2020,3,22),"Si","No")</f>
         <v>No</v>
@@ -13240,7 +13241,7 @@
         <v>Si</v>
       </c>
       <c r="K285" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L285" t="str">
         <f>IF(C285&gt;DATE(2020,3,15),IF(C285&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -13280,7 +13281,7 @@
         <v>Si</v>
       </c>
       <c r="K286" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L286" t="str">
         <f>IF(C286&gt;DATE(2020,3,15),IF(C286&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -13320,7 +13321,7 @@
         <v>Si</v>
       </c>
       <c r="K287" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L287" t="str">
         <f>IF(C287&gt;DATE(2020,3,15),IF(C287&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -13773,28 +13774,27 @@
       </c>
     </row>
     <row r="301" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A301" s="1" t="s">
+      <c r="A301" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B301">
+      <c r="B301" s="18">
         <v>12</v>
       </c>
       <c r="C301" s="3">
         <v>43908</v>
       </c>
-      <c r="D301" s="9">
+      <c r="D301" s="18">
         <v>453</v>
       </c>
-      <c r="E301">
-        <v>16.739999999999998</v>
-      </c>
-      <c r="G301" s="9">
+      <c r="E301" s="19">
+        <v>17</v>
+      </c>
+      <c r="G301" s="18">
         <v>15</v>
       </c>
-      <c r="H301" s="9">
+      <c r="H301" s="18">
         <v>4</v>
       </c>
-      <c r="I301" s="3"/>
       <c r="J301" t="str">
         <f>IF(C301&gt;DATE(2020,3,22),"Si","No")</f>
         <v>No</v>
@@ -14191,7 +14191,7 @@
         <v>Si</v>
       </c>
       <c r="K311" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L311" t="str">
         <f>IF(C311&gt;DATE(2020,3,15),IF(C311&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -14231,7 +14231,7 @@
         <v>Si</v>
       </c>
       <c r="K312" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L312" t="str">
         <f>IF(C312&gt;DATE(2020,3,15),IF(C312&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -14271,7 +14271,7 @@
         <v>Si</v>
       </c>
       <c r="K313" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L313" t="str">
         <f>IF(C313&gt;DATE(2020,3,15),IF(C313&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -14724,28 +14724,27 @@
       </c>
     </row>
     <row r="327" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A327" t="s">
+      <c r="A327" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B327">
+      <c r="B327" s="18">
         <v>13</v>
       </c>
       <c r="C327" s="3">
         <v>43908</v>
       </c>
-      <c r="D327" s="9">
+      <c r="D327" s="19">
         <v>6777</v>
       </c>
-      <c r="E327">
-        <v>100.35</v>
-      </c>
-      <c r="G327" s="9">
+      <c r="E327" s="19">
+        <v>100</v>
+      </c>
+      <c r="G327" s="18">
         <v>590</v>
       </c>
-      <c r="H327" s="9">
+      <c r="H327" s="19">
         <v>498</v>
       </c>
-      <c r="I327" s="3"/>
       <c r="J327" t="str">
         <f>IF(C327&gt;DATE(2020,3,22),"Si","No")</f>
         <v>No</v>
@@ -15142,7 +15141,7 @@
         <v>Si</v>
       </c>
       <c r="K337" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L337" t="str">
         <f>IF(C337&gt;DATE(2020,3,15),IF(C337&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -15182,7 +15181,7 @@
         <v>Si</v>
       </c>
       <c r="K338" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L338" t="str">
         <f>IF(C338&gt;DATE(2020,3,15),IF(C338&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -15222,7 +15221,7 @@
         <v>Si</v>
       </c>
       <c r="K339" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L339" t="str">
         <f>IF(C339&gt;DATE(2020,3,15),IF(C339&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -15675,28 +15674,27 @@
       </c>
     </row>
     <row r="353" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A353" t="s">
+      <c r="A353" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B353">
+      <c r="B353" s="18">
         <v>14</v>
       </c>
       <c r="C353" s="3">
         <v>43908</v>
       </c>
-      <c r="D353" s="9">
+      <c r="D353" s="19">
         <v>167</v>
       </c>
-      <c r="E353">
-        <v>11.18</v>
-      </c>
-      <c r="G353" s="9">
+      <c r="E353" s="19">
+        <v>11</v>
+      </c>
+      <c r="G353" s="19">
         <v>6</v>
       </c>
-      <c r="H353" s="9">
-        <v>0</v>
-      </c>
-      <c r="I353" s="3"/>
+      <c r="H353" s="18">
+        <v>0</v>
+      </c>
       <c r="J353" t="str">
         <f>IF(C353&gt;DATE(2020,3,22),"Si","No")</f>
         <v>No</v>
@@ -16093,7 +16091,7 @@
         <v>Si</v>
       </c>
       <c r="K363" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L363" t="str">
         <f>IF(C363&gt;DATE(2020,3,15),IF(C363&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -16133,7 +16131,7 @@
         <v>Si</v>
       </c>
       <c r="K364" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L364" t="str">
         <f>IF(C364&gt;DATE(2020,3,15),IF(C364&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -16173,7 +16171,7 @@
         <v>Si</v>
       </c>
       <c r="K365" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L365" t="str">
         <f>IF(C365&gt;DATE(2020,3,15),IF(C365&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -16626,28 +16624,27 @@
       </c>
     </row>
     <row r="379" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A379" s="1" t="s">
+      <c r="A379" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B379">
+      <c r="B379" s="18">
         <v>15</v>
       </c>
       <c r="C379" s="3">
         <v>43908</v>
       </c>
-      <c r="D379" s="9">
+      <c r="D379" s="19">
         <v>482</v>
       </c>
-      <c r="E379">
-        <v>73.22</v>
-      </c>
-      <c r="G379" s="9">
+      <c r="E379" s="19">
+        <v>73</v>
+      </c>
+      <c r="G379" s="18">
         <v>11</v>
       </c>
-      <c r="H379" s="9">
+      <c r="H379" s="18">
         <v>4</v>
       </c>
-      <c r="I379" s="3"/>
       <c r="J379" t="str">
         <f>IF(C379&gt;DATE(2020,3,22),"Si","No")</f>
         <v>No</v>
@@ -17044,7 +17041,7 @@
         <v>Si</v>
       </c>
       <c r="K389" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L389" t="str">
         <f>IF(C389&gt;DATE(2020,3,15),IF(C389&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -17084,7 +17081,7 @@
         <v>Si</v>
       </c>
       <c r="K390" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L390" t="str">
         <f>IF(C390&gt;DATE(2020,3,15),IF(C390&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -17124,7 +17121,7 @@
         <v>Si</v>
       </c>
       <c r="K391" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L391" t="str">
         <f>IF(C391&gt;DATE(2020,3,15),IF(C391&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -17577,28 +17574,27 @@
       </c>
     </row>
     <row r="405" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A405" t="s">
+      <c r="A405" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B405">
+      <c r="B405" s="18">
         <v>16</v>
       </c>
       <c r="C405" s="3">
         <v>43908</v>
       </c>
-      <c r="D405" s="9">
+      <c r="D405" s="19">
         <v>1190</v>
       </c>
-      <c r="E405">
-        <v>53.13</v>
-      </c>
-      <c r="G405" s="9">
+      <c r="E405" s="19">
+        <v>53</v>
+      </c>
+      <c r="G405" s="18">
         <v>44</v>
       </c>
-      <c r="H405" s="9">
+      <c r="H405" s="19">
         <v>53</v>
       </c>
-      <c r="I405" s="3"/>
       <c r="J405" t="str">
         <f>IF(C405&gt;DATE(2020,3,22),"Si","No")</f>
         <v>No</v>
@@ -17995,7 +17991,7 @@
         <v>Si</v>
       </c>
       <c r="K415" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L415" t="str">
         <f>IF(C415&gt;DATE(2020,3,15),IF(C415&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -18035,7 +18031,7 @@
         <v>Si</v>
       </c>
       <c r="K416" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L416" t="str">
         <f>IF(C416&gt;DATE(2020,3,15),IF(C416&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -18075,7 +18071,7 @@
         <v>Si</v>
       </c>
       <c r="K417" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L417" t="str">
         <f>IF(C417&gt;DATE(2020,3,15),IF(C417&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -18528,28 +18524,27 @@
       </c>
     </row>
     <row r="431" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A431" s="8" t="s">
+      <c r="A431" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B431">
+      <c r="B431" s="18">
         <v>17</v>
       </c>
       <c r="C431" s="3">
         <v>43908</v>
       </c>
-      <c r="D431" s="9">
+      <c r="D431" s="18">
         <v>468</v>
       </c>
-      <c r="E431">
-        <v>144.26</v>
-      </c>
-      <c r="G431" s="9">
+      <c r="E431" s="18">
+        <v>144.30000000000001</v>
+      </c>
+      <c r="G431" s="18">
         <v>15</v>
       </c>
-      <c r="H431" s="9">
+      <c r="H431" s="18">
         <v>5</v>
       </c>
-      <c r="I431" s="3"/>
       <c r="J431" t="str">
         <f>IF(C431&gt;DATE(2020,3,22),"Si","No")</f>
         <v>No</v>
@@ -18946,7 +18941,7 @@
         <v>Si</v>
       </c>
       <c r="K441" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L441" t="str">
         <f>IF(C441&gt;DATE(2020,3,15),IF(C441&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -18986,7 +18981,7 @@
         <v>Si</v>
       </c>
       <c r="K442" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L442" t="str">
         <f>IF(C442&gt;DATE(2020,3,15),IF(C442&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -19026,7 +19021,7 @@
         <v>Si</v>
       </c>
       <c r="K443" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L443" t="str">
         <f>IF(C443&gt;DATE(2020,3,15),IF(C443&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -19061,7 +19056,7 @@
         <v>No</v>
       </c>
       <c r="K444" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L444" t="str">
         <f>IF(C444&gt;DATE(2020,3,15),IF(C444&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -19096,7 +19091,7 @@
         <v>No</v>
       </c>
       <c r="K445" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L445" t="str">
         <f>IF(C445&gt;DATE(2020,3,15),IF(C445&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -19131,7 +19126,7 @@
         <v>No</v>
       </c>
       <c r="K446" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L446" t="str">
         <f>IF(C446&gt;DATE(2020,3,15),IF(C446&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -19166,7 +19161,7 @@
         <v>No</v>
       </c>
       <c r="K447" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L447" t="str">
         <f>IF(C447&gt;DATE(2020,3,15),IF(C447&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -19201,7 +19196,7 @@
         <v>No</v>
       </c>
       <c r="K448" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L448" t="str">
         <f>IF(C448&gt;DATE(2020,3,15),IF(C448&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -19236,7 +19231,7 @@
         <v>No</v>
       </c>
       <c r="K449" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L449" t="str">
         <f>IF(C449&gt;DATE(2020,3,15),IF(C449&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -19271,7 +19266,7 @@
         <v>No</v>
       </c>
       <c r="K450" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L450" t="str">
         <f>IF(C450&gt;DATE(2020,3,15),IF(C450&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -19306,7 +19301,7 @@
         <v>No</v>
       </c>
       <c r="K451" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L451" t="str">
         <f>IF(C451&gt;DATE(2020,3,15),IF(C451&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -19336,7 +19331,7 @@
         <v>No</v>
       </c>
       <c r="K452" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L452" t="str">
         <f>IF(C452&gt;DATE(2020,3,15),IF(C452&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -19366,7 +19361,7 @@
         <v>No</v>
       </c>
       <c r="K453" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L453" t="str">
         <f>IF(C453&gt;DATE(2020,3,15),IF(C453&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -19401,7 +19396,7 @@
         <v>No</v>
       </c>
       <c r="K454" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L454" t="str">
         <f>IF(C454&gt;DATE(2020,3,15),IF(C454&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -19436,7 +19431,7 @@
         <v>No</v>
       </c>
       <c r="K455" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L455" t="str">
         <f>IF(C455&gt;DATE(2020,3,15),IF(C455&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -19471,7 +19466,7 @@
         <v>No</v>
       </c>
       <c r="K456" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L456" t="str">
         <f>IF(C456&gt;DATE(2020,3,15),IF(C456&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -19479,28 +19474,27 @@
       </c>
     </row>
     <row r="457" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A457" t="s">
+      <c r="A457" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B457">
+      <c r="B457" s="18">
         <v>18</v>
       </c>
       <c r="C457" s="3">
         <v>43908</v>
       </c>
-      <c r="D457" s="9">
+      <c r="D457" s="19">
         <v>1</v>
       </c>
-      <c r="E457">
+      <c r="E457" s="18">
         <v>1.18</v>
       </c>
-      <c r="G457" s="9">
-        <v>0</v>
-      </c>
-      <c r="H457" s="9">
-        <v>0</v>
-      </c>
-      <c r="I457" s="3"/>
+      <c r="G457" s="18">
+        <v>0</v>
+      </c>
+      <c r="H457" s="18">
+        <v>0</v>
+      </c>
       <c r="J457" t="str">
         <f>IF(C457&gt;DATE(2020,3,22),"Si","No")</f>
         <v>No</v>
@@ -19540,7 +19534,7 @@
         <v>No</v>
       </c>
       <c r="K458" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L458" t="str">
         <f>IF(C458&gt;DATE(2020,3,15),IF(C458&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -19577,7 +19571,7 @@
         <v>No</v>
       </c>
       <c r="K459" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L459" t="str">
         <f>IF(C459&gt;DATE(2020,3,15),IF(C459&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -19614,7 +19608,7 @@
         <v>No</v>
       </c>
       <c r="K460" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L460" t="str">
         <f>IF(C460&gt;DATE(2020,3,15),IF(C460&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -19654,7 +19648,7 @@
         <v>No</v>
       </c>
       <c r="K461" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L461" t="str">
         <f>IF(C461&gt;DATE(2020,3,15),IF(C461&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -19694,7 +19688,7 @@
         <v>Si</v>
       </c>
       <c r="K462" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L462" t="str">
         <f>IF(C462&gt;DATE(2020,3,15),IF(C462&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -19734,7 +19728,7 @@
         <v>Si</v>
       </c>
       <c r="K463" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L463" t="str">
         <f>IF(C463&gt;DATE(2020,3,15),IF(C463&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -19774,7 +19768,7 @@
         <v>Si</v>
       </c>
       <c r="K464" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L464" t="str">
         <f>IF(C464&gt;DATE(2020,3,15),IF(C464&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -19814,7 +19808,7 @@
         <v>Si</v>
       </c>
       <c r="K465" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L465" t="str">
         <f>IF(C465&gt;DATE(2020,3,15),IF(C465&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -19854,7 +19848,7 @@
         <v>Si</v>
       </c>
       <c r="K466" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L466" t="str">
         <f>IF(C466&gt;DATE(2020,3,15),IF(C466&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -20008,7 +20002,7 @@
         <v>No</v>
       </c>
       <c r="K470" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L470" t="str">
         <f>IF(C470&gt;DATE(2020,3,15),IF(C470&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -20042,7 +20036,7 @@
         <v>No</v>
       </c>
       <c r="K471" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L471" t="str">
         <f>IF(C471&gt;DATE(2020,3,15),IF(C471&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -20076,7 +20070,7 @@
         <v>No</v>
       </c>
       <c r="K472" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L472" t="str">
         <f>IF(C472&gt;DATE(2020,3,15),IF(C472&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -20110,7 +20104,7 @@
         <v>No</v>
       </c>
       <c r="K473" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L473" t="str">
         <f>IF(C473&gt;DATE(2020,3,15),IF(C473&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -20144,7 +20138,7 @@
         <v>No</v>
       </c>
       <c r="K474" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L474" t="str">
         <f>IF(C474&gt;DATE(2020,3,15),IF(C474&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -20178,7 +20172,7 @@
         <v>No</v>
       </c>
       <c r="K475" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L475" t="str">
         <f>IF(C475&gt;DATE(2020,3,15),IF(C475&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -20212,7 +20206,7 @@
         <v>No</v>
       </c>
       <c r="K476" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L476" t="str">
         <f>IF(C476&gt;DATE(2020,3,15),IF(C476&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -20246,7 +20240,7 @@
         <v>No</v>
       </c>
       <c r="K477" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L477" t="str">
         <f>IF(C477&gt;DATE(2020,3,15),IF(C477&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -20275,7 +20269,7 @@
         <v>No</v>
       </c>
       <c r="K478" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L478" t="str">
         <f>IF(C478&gt;DATE(2020,3,15),IF(C478&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -20304,7 +20298,7 @@
         <v>No</v>
       </c>
       <c r="K479" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L479" t="str">
         <f>IF(C479&gt;DATE(2020,3,15),IF(C479&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -20338,7 +20332,7 @@
         <v>No</v>
       </c>
       <c r="K480" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L480" t="str">
         <f>IF(C480&gt;DATE(2020,3,15),IF(C480&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -20372,7 +20366,7 @@
         <v>No</v>
       </c>
       <c r="K481" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L481" t="str">
         <f>IF(C481&gt;DATE(2020,3,15),IF(C481&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -20406,7 +20400,7 @@
         <v>No</v>
       </c>
       <c r="K482" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L482" t="str">
         <f>IF(C482&gt;DATE(2020,3,15),IF(C482&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -20414,25 +20408,25 @@
       </c>
     </row>
     <row r="483" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A483" s="1" t="s">
+      <c r="A483" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B483">
+      <c r="B483" s="18">
         <v>19</v>
       </c>
       <c r="C483" s="3">
         <v>43908</v>
       </c>
-      <c r="D483" s="9">
+      <c r="D483" s="19">
         <v>23</v>
       </c>
-      <c r="E483">
-        <v>26.59</v>
-      </c>
-      <c r="G483" s="9">
-        <v>0</v>
-      </c>
-      <c r="H483" s="9">
+      <c r="E483" s="19">
+        <v>27</v>
+      </c>
+      <c r="G483" s="18">
+        <v>0</v>
+      </c>
+      <c r="H483" s="18">
         <v>0</v>
       </c>
       <c r="J483" t="str">
@@ -20474,7 +20468,7 @@
         <v>No</v>
       </c>
       <c r="K484" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L484" t="str">
         <f>IF(C484&gt;DATE(2020,3,15),IF(C484&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -20511,7 +20505,7 @@
         <v>No</v>
       </c>
       <c r="K485" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L485" t="str">
         <f>IF(C485&gt;DATE(2020,3,15),IF(C485&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -20548,7 +20542,7 @@
         <v>No</v>
       </c>
       <c r="K486" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L486" t="str">
         <f>IF(C486&gt;DATE(2020,3,15),IF(C486&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -20588,7 +20582,7 @@
         <v>No</v>
       </c>
       <c r="K487" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L487" t="str">
         <f>IF(C487&gt;DATE(2020,3,15),IF(C487&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -20628,7 +20622,7 @@
         <v>Si</v>
       </c>
       <c r="K488" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L488" t="str">
         <f>IF(C488&gt;DATE(2020,3,15),IF(C488&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -20668,7 +20662,7 @@
         <v>Si</v>
       </c>
       <c r="K489" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L489" t="str">
         <f>IF(C489&gt;DATE(2020,3,15),IF(C489&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -20708,7 +20702,7 @@
         <v>Si</v>
       </c>
       <c r="K490" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L490" t="str">
         <f>IF(C490&gt;DATE(2020,3,15),IF(C490&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -20748,7 +20742,7 @@
         <v>Si</v>
       </c>
       <c r="K491" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L491" t="str">
         <f>IF(C491&gt;DATE(2020,3,15),IF(C491&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -20788,7 +20782,7 @@
         <v>Si</v>
       </c>
       <c r="K492" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L492" t="str">
         <f>IF(C492&gt;DATE(2020,3,15),IF(C492&gt;DATE(2020,3,22),"Fuerte","Debil"),"No")</f>
@@ -20916,10 +20910,9 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I343" xr:uid="{EEFE7D21-3722-C547-BC90-A911F1DEF0E0}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I343">
-      <sortCondition ref="A2:A343"/>
-      <sortCondition ref="C2:C343"/>
+  <autoFilter ref="A1:I476" xr:uid="{EEFE7D21-3722-C547-BC90-A911F1DEF0E0}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I476">
+      <sortCondition ref="C1:C476"/>
     </sortState>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L495">
@@ -21977,7 +21970,7 @@
   <dimension ref="A1:U49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:I20"/>
+      <selection activeCell="G2" sqref="A2:G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21991,10 +21984,11 @@
     <col min="7" max="7" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="11" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="21" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="21" width="5.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
@@ -22034,25 +22028,19 @@
         <v>1</v>
       </c>
       <c r="C2" s="16">
-        <v>43920</v>
+        <v>43908</v>
       </c>
       <c r="D2" s="2">
-        <v>5818</v>
+        <v>1008</v>
       </c>
       <c r="E2" s="2">
-        <v>61.03</v>
-      </c>
-      <c r="F2" s="2">
-        <v>2867</v>
+        <v>11.84</v>
+      </c>
+      <c r="F2">
+        <v>25</v>
       </c>
       <c r="G2" s="2">
-        <v>235</v>
-      </c>
-      <c r="H2">
-        <v>248</v>
-      </c>
-      <c r="I2">
-        <v>160</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -22063,25 +22051,19 @@
         <v>2</v>
       </c>
       <c r="C3" s="16">
-        <v>43920</v>
+        <v>43908</v>
       </c>
       <c r="D3" s="2">
-        <v>2272</v>
+        <v>281</v>
       </c>
       <c r="E3" s="2">
-        <v>156.52000000000001</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1176</v>
-      </c>
-      <c r="G3" s="2">
-        <v>165</v>
-      </c>
-      <c r="H3">
-        <v>138</v>
-      </c>
-      <c r="I3">
-        <v>204</v>
+        <v>21.22</v>
+      </c>
+      <c r="F3">
+        <v>14</v>
+      </c>
+      <c r="G3">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -22092,26 +22074,21 @@
         <v>3</v>
       </c>
       <c r="C4" s="16">
-        <v>43920</v>
+        <v>43908</v>
       </c>
       <c r="D4" s="2">
-        <v>1236</v>
-      </c>
-      <c r="E4" s="2">
-        <v>101.97</v>
-      </c>
-      <c r="F4" s="2">
-        <v>529</v>
+        <v>292</v>
+      </c>
+      <c r="E4">
+        <v>28.06</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
       </c>
       <c r="G4">
-        <v>65</v>
-      </c>
-      <c r="H4" s="2">
-        <v>55</v>
-      </c>
-      <c r="I4">
-        <v>90</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H4" s="2"/>
       <c r="M4" t="s">
         <v>52</v>
       </c>
@@ -22124,25 +22101,19 @@
         <v>4</v>
       </c>
       <c r="C5" s="16">
-        <v>43920</v>
+        <v>43908</v>
       </c>
       <c r="D5" s="2">
-        <v>1069</v>
-      </c>
-      <c r="E5" s="2">
-        <v>85</v>
-      </c>
-      <c r="F5" s="2">
-        <v>399</v>
+        <v>169</v>
+      </c>
+      <c r="E5">
+        <v>14.18</v>
+      </c>
+      <c r="F5">
+        <v>7</v>
       </c>
       <c r="G5">
-        <v>85</v>
-      </c>
-      <c r="H5">
-        <v>42</v>
-      </c>
-      <c r="I5">
-        <v>111</v>
+        <v>2</v>
       </c>
       <c r="M5" t="s">
         <v>50</v>
@@ -22156,25 +22127,19 @@
         <v>5</v>
       </c>
       <c r="C6" s="16">
-        <v>43920</v>
+        <v>43908</v>
       </c>
       <c r="D6" s="2">
-        <v>1262</v>
+        <v>220</v>
       </c>
       <c r="E6" s="2">
-        <v>51.73</v>
-      </c>
-      <c r="F6">
-        <v>483</v>
+        <v>9.84</v>
+      </c>
+      <c r="F6" s="2">
+        <v>23</v>
       </c>
       <c r="G6">
-        <v>94</v>
-      </c>
-      <c r="H6">
-        <v>55</v>
-      </c>
-      <c r="I6">
-        <v>57</v>
+        <v>3</v>
       </c>
       <c r="M6" t="s">
         <v>49</v>
@@ -22188,25 +22153,19 @@
         <v>6</v>
       </c>
       <c r="C7" s="16">
-        <v>43920</v>
+        <v>43908</v>
       </c>
       <c r="D7" s="2">
-        <v>1171</v>
+        <v>83</v>
       </c>
       <c r="E7" s="2">
-        <v>191.54</v>
-      </c>
-      <c r="F7">
-        <v>522</v>
+        <v>12.56</v>
+      </c>
+      <c r="F7" s="2">
+        <v>4</v>
       </c>
       <c r="G7">
-        <v>50</v>
-      </c>
-      <c r="H7">
-        <v>37</v>
-      </c>
-      <c r="I7">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="M7" t="s">
         <v>51</v>
@@ -22220,25 +22179,19 @@
         <v>8</v>
       </c>
       <c r="C8" s="16">
-        <v>43920</v>
+        <v>43908</v>
       </c>
       <c r="D8" s="2">
-        <v>6424</v>
+        <v>801</v>
       </c>
       <c r="E8" s="2">
-        <v>288.12</v>
+        <v>38.76</v>
       </c>
       <c r="F8" s="2">
-        <v>3225</v>
+        <v>37</v>
       </c>
       <c r="G8" s="2">
-        <v>344</v>
-      </c>
-      <c r="H8">
-        <v>708</v>
-      </c>
-      <c r="I8">
-        <v>296</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -22249,26 +22202,21 @@
         <v>7</v>
       </c>
       <c r="C9" s="16">
-        <v>43920</v>
-      </c>
-      <c r="D9" s="2">
-        <v>6211</v>
+        <v>43908</v>
+      </c>
+      <c r="D9">
+        <v>868</v>
       </c>
       <c r="E9" s="2">
-        <v>240.88</v>
-      </c>
-      <c r="F9" s="2">
-        <v>2601</v>
+        <v>35.72</v>
+      </c>
+      <c r="F9">
+        <v>54</v>
       </c>
       <c r="G9" s="2">
-        <v>325</v>
-      </c>
-      <c r="H9">
-        <v>516</v>
-      </c>
-      <c r="I9" s="2">
-        <v>1028</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -22278,26 +22226,22 @@
         <v>9</v>
       </c>
       <c r="C10" s="16">
-        <v>43920</v>
+        <v>43908</v>
       </c>
       <c r="D10" s="2">
-        <v>18773</v>
+        <v>2702</v>
       </c>
       <c r="E10" s="2">
-        <v>226.43</v>
+        <v>34.89</v>
       </c>
       <c r="F10" s="2">
-        <v>12974</v>
+        <v>33</v>
       </c>
       <c r="G10" s="2">
-        <v>1652</v>
-      </c>
-      <c r="H10" s="2">
-        <v>1672</v>
-      </c>
-      <c r="I10" s="2">
-        <v>4966</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -22308,26 +22252,21 @@
         <v>18</v>
       </c>
       <c r="C11" s="16">
-        <v>43920</v>
-      </c>
-      <c r="D11">
-        <v>34</v>
+        <v>43908</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>38.93</v>
-      </c>
-      <c r="F11" s="2">
-        <v>3</v>
+        <v>1.18</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>3</v>
-      </c>
-      <c r="H11" s="2">
-        <v>1</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H11" s="2"/>
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
@@ -22338,26 +22277,22 @@
         <v>10</v>
       </c>
       <c r="C12" s="16">
-        <v>43920</v>
+        <v>43908</v>
       </c>
       <c r="D12" s="2">
-        <v>5508</v>
+        <v>921</v>
       </c>
       <c r="E12" s="2">
-        <v>99.27</v>
+        <v>18.03</v>
       </c>
       <c r="F12" s="2">
-        <v>2189</v>
+        <v>52</v>
       </c>
       <c r="G12" s="2">
-        <v>356</v>
-      </c>
-      <c r="H12" s="2">
-        <v>339</v>
-      </c>
-      <c r="I12" s="2">
-        <v>200</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -22367,25 +22302,19 @@
         <v>11</v>
       </c>
       <c r="C13" s="16">
-        <v>43920</v>
+        <v>43908</v>
       </c>
       <c r="D13" s="2">
-        <v>1628</v>
+        <v>241</v>
       </c>
       <c r="E13" s="2">
-        <v>138.15</v>
-      </c>
-      <c r="F13">
-        <v>371</v>
-      </c>
-      <c r="G13">
-        <v>51</v>
-      </c>
-      <c r="H13">
-        <v>133</v>
-      </c>
-      <c r="I13">
-        <v>91</v>
+        <v>22.01</v>
+      </c>
+      <c r="F13" s="2">
+        <v>3</v>
+      </c>
+      <c r="G13" s="2">
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
@@ -22396,26 +22325,21 @@
         <v>12</v>
       </c>
       <c r="C14" s="16">
-        <v>43920</v>
-      </c>
-      <c r="D14" s="2">
-        <v>4039</v>
+        <v>43908</v>
+      </c>
+      <c r="D14">
+        <v>453</v>
       </c>
       <c r="E14" s="2">
-        <v>138.80000000000001</v>
-      </c>
-      <c r="F14" s="2">
-        <v>1250</v>
-      </c>
-      <c r="G14" s="2">
-        <v>149</v>
-      </c>
-      <c r="H14" s="2">
-        <v>84</v>
-      </c>
-      <c r="I14">
-        <v>187</v>
-      </c>
+        <v>16.739999999999998</v>
+      </c>
+      <c r="F14">
+        <v>15</v>
+      </c>
+      <c r="G14">
+        <v>4</v>
+      </c>
+      <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -22425,26 +22349,22 @@
         <v>13</v>
       </c>
       <c r="C15" s="16">
-        <v>43920</v>
+        <v>43908</v>
       </c>
       <c r="D15" s="2">
-        <v>27509</v>
+        <v>6777</v>
       </c>
       <c r="E15" s="2">
-        <v>339.74</v>
-      </c>
-      <c r="F15" s="2">
-        <v>15140</v>
+        <v>100.35</v>
+      </c>
+      <c r="F15">
+        <v>590</v>
       </c>
       <c r="G15" s="2">
-        <v>1514</v>
-      </c>
-      <c r="H15" s="2">
-        <v>3603</v>
-      </c>
-      <c r="I15" s="2">
-        <v>9330</v>
-      </c>
+        <v>498</v>
+      </c>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -22455,24 +22375,18 @@
         <v>19</v>
       </c>
       <c r="C16" s="16">
-        <v>43920</v>
-      </c>
-      <c r="D16">
-        <v>54</v>
-      </c>
-      <c r="E16">
-        <v>42.78</v>
-      </c>
-      <c r="F16" s="2">
-        <v>27</v>
+        <v>43908</v>
+      </c>
+      <c r="D16" s="2">
+        <v>23</v>
+      </c>
+      <c r="E16" s="2">
+        <v>26.59</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
       </c>
       <c r="G16">
-        <v>3</v>
-      </c>
-      <c r="H16">
-        <v>1</v>
-      </c>
-      <c r="I16">
         <v>0</v>
       </c>
       <c r="J16" s="2"/>
@@ -22485,26 +22399,22 @@
         <v>14</v>
       </c>
       <c r="C17" s="16">
-        <v>43920</v>
-      </c>
-      <c r="D17">
-        <v>974</v>
-      </c>
-      <c r="E17">
-        <v>58.71</v>
+        <v>43908</v>
+      </c>
+      <c r="D17" s="2">
+        <v>167</v>
+      </c>
+      <c r="E17" s="2">
+        <v>11.18</v>
       </c>
       <c r="F17" s="2">
-        <v>283</v>
+        <v>6</v>
       </c>
       <c r="G17">
-        <v>59</v>
-      </c>
-      <c r="H17" s="2">
-        <v>34</v>
-      </c>
-      <c r="I17" s="2">
-        <v>20</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
@@ -22514,25 +22424,19 @@
         <v>15</v>
       </c>
       <c r="C18" s="16">
-        <v>43920</v>
+        <v>43908</v>
       </c>
       <c r="D18" s="2">
-        <v>2305</v>
+        <v>482</v>
       </c>
       <c r="E18" s="2">
-        <v>304.49</v>
-      </c>
-      <c r="F18" s="2">
-        <v>1035</v>
+        <v>73.22</v>
+      </c>
+      <c r="F18">
+        <v>11</v>
       </c>
       <c r="G18">
-        <v>99</v>
-      </c>
-      <c r="H18">
-        <v>113</v>
-      </c>
-      <c r="I18">
-        <v>192</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.2">
@@ -22543,26 +22447,21 @@
         <v>16</v>
       </c>
       <c r="C19" s="16">
-        <v>43920</v>
+        <v>43908</v>
       </c>
       <c r="D19" s="2">
-        <v>6320</v>
+        <v>1190</v>
       </c>
       <c r="E19" s="2">
-        <v>251.61</v>
-      </c>
-      <c r="F19" s="2">
-        <v>3594</v>
+        <v>53.13</v>
+      </c>
+      <c r="F19">
+        <v>44</v>
       </c>
       <c r="G19" s="2">
-        <v>307</v>
-      </c>
-      <c r="H19">
-        <v>325</v>
-      </c>
-      <c r="I19" s="2">
-        <v>1796</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="I19" s="2"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
@@ -22572,25 +22471,19 @@
         <v>17</v>
       </c>
       <c r="C20" s="16">
-        <v>43920</v>
-      </c>
-      <c r="D20" s="2">
-        <v>1810</v>
-      </c>
-      <c r="E20" s="2">
-        <v>459.28</v>
-      </c>
-      <c r="F20" s="2">
-        <v>575</v>
+        <v>43908</v>
+      </c>
+      <c r="D20">
+        <v>468</v>
+      </c>
+      <c r="E20">
+        <v>144.26</v>
+      </c>
+      <c r="F20">
+        <v>15</v>
       </c>
       <c r="G20">
-        <v>51</v>
-      </c>
-      <c r="H20">
-        <v>85</v>
-      </c>
-      <c r="I20">
-        <v>496</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.2">
@@ -22608,170 +22501,106 @@
       <c r="B23" s="1"/>
       <c r="E23" s="2"/>
       <c r="G23" s="2"/>
-      <c r="L23" t="s">
-        <v>57</v>
-      </c>
-      <c r="M23" s="2">
-        <v>5818</v>
-      </c>
-      <c r="N23" s="2">
-        <v>61.03</v>
-      </c>
-      <c r="O23" s="2">
-        <v>2867</v>
-      </c>
-      <c r="P23" s="2">
-        <v>235</v>
-      </c>
-      <c r="Q23">
-        <v>248</v>
-      </c>
-      <c r="R23">
-        <v>160</v>
-      </c>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="E24" s="2"/>
-      <c r="L24" t="s">
-        <v>58</v>
-      </c>
-      <c r="M24" s="2">
-        <v>2272</v>
-      </c>
-      <c r="N24" s="2">
-        <v>156.52000000000001</v>
-      </c>
-      <c r="O24" s="2">
-        <v>1176</v>
-      </c>
-      <c r="P24" s="2">
-        <v>165</v>
-      </c>
-      <c r="Q24">
-        <v>138</v>
-      </c>
-      <c r="R24">
-        <v>204</v>
-      </c>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="L25" t="s">
-        <v>12</v>
-      </c>
-      <c r="M25" s="2">
-        <v>1236</v>
+      <c r="M25" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="N25" s="2">
-        <v>101.97</v>
+        <v>1008</v>
       </c>
       <c r="O25" s="2">
-        <v>529</v>
+        <v>11.84</v>
       </c>
       <c r="P25">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="Q25" s="2">
-        <v>55</v>
-      </c>
-      <c r="R25">
-        <v>90</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="E26" s="2"/>
-      <c r="L26" t="s">
-        <v>13</v>
-      </c>
-      <c r="M26" s="2">
-        <v>1069</v>
+      <c r="M26" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="N26" s="2">
-        <v>85</v>
+        <v>281</v>
       </c>
       <c r="O26" s="2">
-        <v>399</v>
+        <v>21.22</v>
       </c>
       <c r="P26">
-        <v>85</v>
+        <v>14</v>
       </c>
       <c r="Q26">
-        <v>42</v>
-      </c>
-      <c r="R26">
-        <v>111</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="L27" t="s">
-        <v>14</v>
-      </c>
-      <c r="M27" s="2">
-        <v>1262</v>
+      <c r="M27" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="N27" s="2">
-        <v>51.73</v>
+        <v>292</v>
       </c>
       <c r="O27">
-        <v>483</v>
+        <v>28.06</v>
       </c>
       <c r="P27">
-        <v>94</v>
+        <v>6</v>
       </c>
       <c r="Q27">
-        <v>55</v>
-      </c>
-      <c r="R27">
-        <v>57</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="E28" s="2"/>
       <c r="G28" s="2"/>
-      <c r="L28" t="s">
-        <v>15</v>
-      </c>
-      <c r="M28" s="2">
-        <v>1171</v>
+      <c r="M28" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="N28" s="2">
-        <v>191.54</v>
+        <v>169</v>
       </c>
       <c r="O28">
-        <v>522</v>
+        <v>14.18</v>
       </c>
       <c r="P28">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="Q28">
-        <v>37</v>
-      </c>
-      <c r="R28">
-        <v>35</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="E29" s="2"/>
       <c r="G29" s="2"/>
-      <c r="L29" t="s">
-        <v>59</v>
-      </c>
-      <c r="M29" s="2">
-        <v>6424</v>
+      <c r="M29" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="N29" s="2">
-        <v>288.12</v>
+        <v>220</v>
       </c>
       <c r="O29" s="2">
-        <v>3225</v>
+        <v>9.84</v>
       </c>
       <c r="P29" s="2">
-        <v>344</v>
+        <v>23</v>
       </c>
       <c r="Q29">
-        <v>708</v>
-      </c>
-      <c r="R29">
-        <v>296</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.2">
@@ -22782,27 +22611,22 @@
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
-      <c r="L30" t="s">
-        <v>60</v>
-      </c>
-      <c r="M30" s="2">
-        <v>6211</v>
+      <c r="M30" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="N30" s="2">
-        <v>240.88</v>
+        <v>83</v>
       </c>
       <c r="O30" s="2">
-        <v>2601</v>
+        <v>12.56</v>
       </c>
       <c r="P30" s="2">
-        <v>325</v>
+        <v>4</v>
       </c>
       <c r="Q30">
-        <v>516</v>
-      </c>
-      <c r="R30" s="2">
-        <v>1028</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="R30" s="2"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B31" s="1"/>
@@ -22811,106 +22635,84 @@
       <c r="H31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
-      <c r="L31" t="s">
-        <v>61</v>
-      </c>
-      <c r="M31" s="2">
-        <v>18773</v>
+      <c r="M31" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="N31" s="2">
-        <v>226.43</v>
+        <v>801</v>
       </c>
       <c r="O31" s="2">
-        <v>12974</v>
+        <v>38.76</v>
       </c>
       <c r="P31" s="2">
-        <v>1652</v>
+        <v>37</v>
       </c>
       <c r="Q31" s="2">
-        <v>1672</v>
-      </c>
-      <c r="R31" s="2">
-        <v>4966</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="R31" s="2"/>
       <c r="S31" s="2"/>
       <c r="T31" s="2"/>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="E32" s="2"/>
       <c r="G32" s="2"/>
-      <c r="L32" t="s">
-        <v>1</v>
-      </c>
-      <c r="M32">
-        <v>34</v>
+      <c r="M32" t="s">
+        <v>59</v>
       </c>
       <c r="N32">
-        <v>38.93</v>
+        <v>868</v>
       </c>
       <c r="O32" s="2">
-        <v>3</v>
+        <v>35.72</v>
       </c>
       <c r="P32">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="Q32" s="2">
-        <v>1</v>
-      </c>
-      <c r="R32">
-        <v>0</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B33" s="1"/>
       <c r="E33" s="2"/>
       <c r="G33" s="2"/>
-      <c r="L33" t="s">
-        <v>2</v>
-      </c>
-      <c r="M33" s="2">
-        <v>5508</v>
+      <c r="M33" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="N33" s="2">
-        <v>99.27</v>
+        <v>2702</v>
       </c>
       <c r="O33" s="2">
-        <v>2189</v>
+        <v>34.89</v>
       </c>
       <c r="P33" s="2">
-        <v>356</v>
+        <v>33</v>
       </c>
       <c r="Q33" s="2">
-        <v>339</v>
-      </c>
-      <c r="R33" s="2">
-        <v>200</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="R33" s="2"/>
       <c r="T33" s="2"/>
       <c r="U33" s="2"/>
     </row>
     <row r="34" spans="2:21" x14ac:dyDescent="0.2">
       <c r="E34" s="2"/>
       <c r="G34" s="2"/>
-      <c r="L34" t="s">
-        <v>3</v>
-      </c>
-      <c r="M34" s="2">
-        <v>1628</v>
+      <c r="M34" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="N34" s="2">
-        <v>138.15</v>
+        <v>1</v>
       </c>
       <c r="O34">
-        <v>371</v>
+        <v>1.18</v>
       </c>
       <c r="P34">
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="Q34">
-        <v>133</v>
-      </c>
-      <c r="R34">
-        <v>91</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="2:21" x14ac:dyDescent="0.2">
@@ -22920,26 +22722,20 @@
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
-      <c r="L35" t="s">
-        <v>4</v>
-      </c>
-      <c r="M35" s="2">
-        <v>4039</v>
+      <c r="M35" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="N35" s="2">
-        <v>138.80000000000001</v>
+        <v>921</v>
       </c>
       <c r="O35" s="2">
-        <v>1250</v>
+        <v>18.03</v>
       </c>
       <c r="P35" s="2">
-        <v>149</v>
+        <v>52</v>
       </c>
       <c r="Q35" s="2">
-        <v>84</v>
-      </c>
-      <c r="R35">
-        <v>187</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36" spans="2:21" x14ac:dyDescent="0.2">
@@ -22950,52 +22746,41 @@
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
-      <c r="L36" t="s">
-        <v>5</v>
-      </c>
-      <c r="M36" s="2">
-        <v>27509</v>
+      <c r="M36" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="N36" s="2">
-        <v>339.74</v>
+        <v>241</v>
       </c>
       <c r="O36" s="2">
-        <v>15140</v>
+        <v>22.01</v>
       </c>
       <c r="P36" s="2">
-        <v>1514</v>
+        <v>3</v>
       </c>
       <c r="Q36" s="2">
-        <v>3603</v>
-      </c>
-      <c r="R36" s="2">
-        <v>9330</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="R36" s="2"/>
       <c r="S36" s="2"/>
       <c r="T36" s="2"/>
     </row>
     <row r="37" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B37" s="2"/>
-      <c r="L37" t="s">
-        <v>6</v>
-      </c>
-      <c r="M37">
-        <v>54</v>
+      <c r="M37" t="s">
+        <v>4</v>
       </c>
       <c r="N37">
-        <v>42.78</v>
+        <v>453</v>
       </c>
       <c r="O37" s="2">
-        <v>27</v>
+        <v>16.739999999999998</v>
       </c>
       <c r="P37">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="Q37">
-        <v>1</v>
-      </c>
-      <c r="R37">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="2:21" x14ac:dyDescent="0.2">
@@ -23003,27 +22788,22 @@
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
-      <c r="L38" t="s">
-        <v>7</v>
-      </c>
-      <c r="M38">
-        <v>974</v>
-      </c>
-      <c r="N38">
-        <v>58.71</v>
+      <c r="M38" t="s">
+        <v>5</v>
+      </c>
+      <c r="N38" s="2">
+        <v>6777</v>
       </c>
       <c r="O38" s="2">
-        <v>283</v>
+        <v>100.35</v>
       </c>
       <c r="P38">
-        <v>59</v>
+        <v>590</v>
       </c>
       <c r="Q38" s="2">
-        <v>34</v>
-      </c>
-      <c r="R38" s="2">
-        <v>20</v>
-      </c>
+        <v>498</v>
+      </c>
+      <c r="R38" s="2"/>
       <c r="S38" s="2"/>
       <c r="T38" s="2"/>
       <c r="U38" s="2"/>
@@ -23032,53 +22812,42 @@
       <c r="E39" s="2"/>
       <c r="G39" s="2"/>
       <c r="J39" s="2"/>
-      <c r="L39" t="s">
-        <v>8</v>
-      </c>
-      <c r="M39" s="2">
-        <v>2305</v>
+      <c r="M39" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="N39" s="2">
-        <v>304.49</v>
+        <v>23</v>
       </c>
       <c r="O39" s="2">
-        <v>1035</v>
+        <v>26.59</v>
       </c>
       <c r="P39">
-        <v>99</v>
+        <v>0</v>
       </c>
       <c r="Q39">
-        <v>113</v>
-      </c>
-      <c r="R39">
-        <v>192</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B40" s="14"/>
       <c r="E40" s="2"/>
       <c r="G40" s="2"/>
-      <c r="L40" t="s">
-        <v>62</v>
-      </c>
-      <c r="M40" s="2">
-        <v>6320</v>
+      <c r="M40" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="N40" s="2">
-        <v>251.61</v>
+        <v>167</v>
       </c>
       <c r="O40" s="2">
-        <v>3594</v>
+        <v>11.18</v>
       </c>
       <c r="P40" s="2">
-        <v>307</v>
+        <v>6</v>
       </c>
       <c r="Q40">
-        <v>325</v>
-      </c>
-      <c r="R40" s="2">
-        <v>1796</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="R40" s="2"/>
       <c r="S40" s="2"/>
     </row>
     <row r="41" spans="2:21" x14ac:dyDescent="0.2">
@@ -23088,32 +22857,39 @@
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
-      <c r="L41" t="s">
-        <v>19</v>
-      </c>
-      <c r="M41" s="2">
-        <v>1810</v>
+      <c r="M41" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="N41" s="2">
-        <v>459.28</v>
+        <v>482</v>
       </c>
       <c r="O41" s="2">
-        <v>575</v>
+        <v>73.22</v>
       </c>
       <c r="P41">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="Q41">
-        <v>85</v>
-      </c>
-      <c r="R41">
-        <v>496</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B42" s="2"/>
-      <c r="O42" s="2"/>
-      <c r="Q42" s="2"/>
+      <c r="M42" t="s">
+        <v>61</v>
+      </c>
+      <c r="N42" s="2">
+        <v>1190</v>
+      </c>
+      <c r="O42" s="2">
+        <v>53.13</v>
+      </c>
+      <c r="P42">
+        <v>44</v>
+      </c>
+      <c r="Q42" s="2">
+        <v>53</v>
+      </c>
     </row>
     <row r="43" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B43" s="2"/>
@@ -23121,6 +22897,21 @@
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
+      <c r="M43" t="s">
+        <v>19</v>
+      </c>
+      <c r="N43">
+        <v>468</v>
+      </c>
+      <c r="O43">
+        <v>144.26</v>
+      </c>
+      <c r="P43">
+        <v>15</v>
+      </c>
+      <c r="Q43">
+        <v>5</v>
+      </c>
     </row>
     <row r="44" spans="2:21" x14ac:dyDescent="0.2">
       <c r="O44" s="2"/>

</xml_diff>